<commit_message>
Continued updating backtesting function
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Trades" sheetId="1" state="visible" r:id="rId1"/>
@@ -73,11 +73,14 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
@@ -460,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
@@ -468,271 +471,347 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="28.48"/>
-    <col customWidth="1" max="2" min="2" style="3" width="8.67"/>
-    <col customWidth="1" max="3" min="3" style="3" width="9.44"/>
-    <col customWidth="1" max="4" min="4" style="3" width="12.1"/>
-    <col customWidth="1" max="5" min="5" style="3" width="12.37"/>
-    <col customWidth="1" max="8" min="6" style="3" width="8.67"/>
-    <col customWidth="1" max="9" min="9" style="3" width="31.96"/>
-    <col customWidth="1" max="1025" min="10" style="3" width="8.67"/>
+    <col customWidth="1" max="1" min="1" style="4" width="28.48"/>
+    <col customWidth="1" max="2" min="2" style="4" width="8.67"/>
+    <col customWidth="1" max="3" min="3" style="4" width="9.44"/>
+    <col customWidth="1" max="4" min="4" style="4" width="12.1"/>
+    <col customWidth="1" max="5" min="5" style="4" width="12.37"/>
+    <col customWidth="1" max="8" min="6" style="4" width="8.67"/>
+    <col customWidth="1" max="9" min="9" style="4" width="31.96"/>
+    <col customWidth="1" max="1025" min="10" style="4" width="8.67"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="13.8" r="1" s="4">
-      <c r="A1" s="3" t="inlineStr">
+    <row customHeight="1" ht="13.8" r="1" s="5">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Stock</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>Bank</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="2" s="4">
-      <c r="A2" s="3" t="inlineStr">
+    <row customHeight="1" ht="13.8" r="2" s="5">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" s="4" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr">
+      <c r="C2" s="4" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="D2" s="3" t="inlineStr">
+      <c r="D2" s="4" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="4" t="n">
         <v>1000</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="3" s="4">
-      <c r="A3" s="5" t="n">
+    <row customHeight="1" ht="15" r="3" s="5">
+      <c r="A3" s="6" t="n">
         <v>44189.90281682289</v>
       </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>NIO</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="n">
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>NIO</t>
+        </is>
+      </c>
+      <c r="C3" s="4" t="n">
         <v>45.7700004577637</v>
       </c>
-      <c r="D3" s="3" t="n">
+      <c r="D3" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="n">
+      <c r="E3" s="4" t="n">
         <v>771.149997711182</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="4" s="4">
-      <c r="A4" s="5" t="n">
+    <row customHeight="1" ht="15" r="4" s="5">
+      <c r="A4" s="6" t="n">
         <v>44189.903063248</v>
       </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>NIO</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="n">
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>NIO</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="n">
         <v>45.7700004577637</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="E4" s="3" t="n">
+      <c r="E4" s="4" t="n">
         <v>542.2999954223631</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="5" s="4">
-      <c r="A5" s="5" t="n">
+    <row customHeight="1" ht="15" r="5" s="5">
+      <c r="A5" s="6" t="n">
         <v>44189.906201055</v>
       </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>NIO</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="n">
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>NIO</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="n">
         <v>45.7700004577637</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="4" t="n">
         <v>313.449993133545</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="6" s="4">
-      <c r="A6" s="5" t="n">
+    <row customHeight="1" ht="15" r="6" s="5">
+      <c r="A6" s="6" t="n">
         <v>44189.9101397843</v>
       </c>
-      <c r="B6" s="3" t="inlineStr">
-        <is>
-          <t>NIO</t>
-        </is>
-      </c>
-      <c r="C6" s="3" t="n">
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>NIO</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="n">
         <v>45.7700004577637</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="E6" s="3" t="n">
+      <c r="E6" s="4" t="n">
         <v>84.59999084472661</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="7" s="4">
-      <c r="A7" s="5" t="n">
+    <row customHeight="1" ht="15" r="7" s="5">
+      <c r="A7" s="6" t="n">
         <v>44189.91564176351</v>
       </c>
-      <c r="B7" s="3" t="inlineStr">
-        <is>
-          <t>NIO</t>
-        </is>
-      </c>
-      <c r="C7" s="3" t="n">
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>NIO</t>
+        </is>
+      </c>
+      <c r="C7" s="4" t="n">
         <v>45.7700004577637</v>
       </c>
-      <c r="D7" s="3" t="n">
+      <c r="D7" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="E7" s="3" t="n">
+      <c r="E7" s="4" t="n">
         <v>38.8299903869629</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="8" s="4">
-      <c r="A8" s="5" t="n">
+    <row customHeight="1" ht="15" r="8" s="5">
+      <c r="A8" s="6" t="n">
         <v>44189.9213225955</v>
       </c>
-      <c r="B8" s="3" t="inlineStr">
-        <is>
-          <t>NIO</t>
-        </is>
-      </c>
-      <c r="C8" s="3" t="n">
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>NIO</t>
+        </is>
+      </c>
+      <c r="C8" s="4" t="n">
         <v>45.7700004577637</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D8" s="4" t="n">
         <v>-100</v>
       </c>
-      <c r="E8" s="3" t="n">
+      <c r="E8" s="4" t="n">
         <v>4615.83003616333</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="9" s="4">
-      <c r="A9" s="5" t="n">
+    <row customHeight="1" ht="15" r="9" s="5">
+      <c r="A9" s="6" t="n">
         <v>44189.9267222921</v>
       </c>
-      <c r="B9" s="3" t="inlineStr">
-        <is>
-          <t>NIO</t>
-        </is>
-      </c>
-      <c r="C9" s="3" t="n">
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>NIO</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="n">
         <v>45.7700004577637</v>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="E9" s="3" t="n">
+      <c r="E9" s="4" t="n">
         <v>38.8299903869629</v>
       </c>
     </row>
-    <row r="10">
+    <row customHeight="1" ht="15" r="10" s="5">
       <c r="A10" s="6" t="n">
-        <v>44189.94454651487</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>NIO</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
+        <v>44189.9445465149</v>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t>NIO</t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>45.7700004577637</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>-20</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>954.23</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="11" s="5">
+      <c r="A11" s="6" t="n">
+        <v>44190.47366530411</v>
+      </c>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t>NIO</t>
+        </is>
+      </c>
+      <c r="C11" s="4" t="n">
+        <v>45.7700004577637</v>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>-20</v>
+      </c>
+      <c r="E11" s="4" t="n">
+        <v>1869.63</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="n">
+        <v>44190.47479848916</v>
+      </c>
+      <c r="B12" s="4" t="inlineStr">
+        <is>
+          <t>NIO</t>
+        </is>
+      </c>
+      <c r="C12" s="4" t="n">
         <v>45.77000045776367</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D12" s="4" t="n">
         <v>-20</v>
       </c>
-      <c r="E10" t="n">
-        <v>954.23</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="12.8" r="1048526" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048527" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048528" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048529" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048530" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048531" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048532" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048533" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048534" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048535" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048536" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048537" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048538" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048539" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048540" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048541" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048542" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048543" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048544" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048545" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048546" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048547" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048548" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048549" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048550" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048551" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048552" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048553" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048554" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048555" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048556" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048557" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048558" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048559" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048560" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048561" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048562" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048563" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048564" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048565" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048566" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048567" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048568" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048569" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048570" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048571" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048572" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048573" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048574" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048575" s="4"/>
-    <row customHeight="1" ht="12.8" r="1048576" s="4"/>
+      <c r="E12" s="4" t="n">
+        <v>2785.03</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="n">
+        <v>44190.47517237271</v>
+      </c>
+      <c r="B13" s="4" t="inlineStr">
+        <is>
+          <t>NIO</t>
+        </is>
+      </c>
+      <c r="C13" s="4" t="n">
+        <v>45.77000045776367</v>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>45</v>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>725.38</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="n">
+        <v>44190.48084385721</v>
+      </c>
+      <c r="B14" s="4" t="inlineStr">
+        <is>
+          <t>NIO</t>
+        </is>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>45.77000045776367</v>
+      </c>
+      <c r="D14" s="4" t="n">
+        <v>-45</v>
+      </c>
+      <c r="E14" s="4" t="n">
+        <v>2785.03</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="1048526" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048527" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048528" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048529" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048530" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048531" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048532" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048533" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048534" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048535" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048536" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048537" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048538" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048539" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048540" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048541" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048542" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048543" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048544" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048545" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048546" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048547" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048548" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048549" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048550" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048551" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048552" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048553" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048554" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048555" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048556" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048557" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048558" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048559" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048560" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048561" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048562" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048563" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048564" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048565" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048566" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048567" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048568" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048569" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048570" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048571" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048572" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048573" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048574" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048575" s="5"/>
+    <row customHeight="1" ht="12.8" r="1048576" s="5"/>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
@@ -746,34 +825,54 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C3" activeCellId="0" pane="topLeft" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="8.67"/>
-    <col customWidth="1" max="2" min="2" style="3" width="18.06"/>
-    <col customWidth="1" max="3" min="3" style="3" width="19.45"/>
-    <col customWidth="1" max="1025" min="4" style="3" width="8.67"/>
+    <col customWidth="1" max="1" min="1" style="4" width="8.67"/>
+    <col customWidth="1" max="2" min="2" style="4" width="18.06"/>
+    <col customWidth="1" max="3" min="3" style="4" width="19.45"/>
+    <col customWidth="1" max="1025" min="4" style="4" width="8.67"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="12.8" r="1" s="4">
-      <c r="A1" s="3" t="inlineStr">
+    <row customHeight="1" ht="12.8" r="1" s="5">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Stock</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Most Recent Buy</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Current Quantity</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="2" s="5">
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>NIO</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="n">
+        <v>44190.48084385721</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="12.8" r="3" s="5">
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <t>TSLA</t>
         </is>
       </c>
     </row>
@@ -800,58 +899,58 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A10" activeCellId="0" pane="topLeft" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="3" width="8.67"/>
-    <col customWidth="1" max="2" min="2" style="3" width="24.87"/>
-    <col customWidth="1" max="1025" min="3" style="3" width="8.67"/>
+    <col customWidth="1" max="1" min="1" style="4" width="8.67"/>
+    <col customWidth="1" max="2" min="2" style="4" width="24.87"/>
+    <col customWidth="1" max="1025" min="3" style="4" width="8.67"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="13.8" r="1" s="4">
-      <c r="A1" s="3" t="inlineStr">
+    <row customHeight="1" ht="13.8" r="1" s="5">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Outside Trading Hours</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="2" s="4">
-      <c r="A2" s="3" t="inlineStr">
+    <row customHeight="1" ht="13.8" r="2" s="5">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>YES</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" s="4" t="inlineStr">
         <is>
           <t>Insufficient Funds</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="3" s="4">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
+    <row customHeight="1" ht="13.8" r="3" s="5">
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
         <is>
           <t>Insufficient Stock Quantity</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="13.8" r="4" s="4">
-      <c r="A4" s="3" t="n">
+    <row customHeight="1" ht="13.8" r="4" s="5">
+      <c r="A4" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="B4" s="3" t="inlineStr">
+      <c r="B4" s="4" t="inlineStr">
         <is>
           <t>Day Trades</t>
         </is>

</xml_diff>